<commit_message>
Updated GA, Main, Utility
</commit_message>
<xml_diff>
--- a/results/Spectrum_Analyzer_20250626.xlsx
+++ b/results/Spectrum_Analyzer_20250626.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:B16"/>
+  <dimension ref="A2:B46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,6 +541,222 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2025-06-26 11:54:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Marker Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Marker Power (dBm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>8.9470000000E+07</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>-1.000000E+03</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-06-26 11:56:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Marker Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Marker Power (dBm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>8.9470000000E+07</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>-1.000000E+03</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-06-26 12:10:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Marker Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Marker Power (dBm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>8.9470000000E+07</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>-1.000000E+03</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2025-06-26 12:14:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Marker Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Marker Power (dBm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2.241600000000E+09</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>-8.8010E+01</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-06-26 12:30:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Marker Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Marker Power (dBm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2.203 GHz</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>-88.88 dBm</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-06-26 12:31:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Marker Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Marker Power (dBm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2.248 GHz</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>-88.99 dBm</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>